<commit_message>
Update with new config excel
</commit_message>
<xml_diff>
--- a/conf/excel/B_China_POI.xlsx
+++ b/conf/excel/B_China_POI.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\配置文件相关\Final-newCA-config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\学习资料\综合学习资料\tencent\配置文件相关\newCA-config-clear\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FA784C-A48A-48AF-88A5-0649004A9D9C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B_China_POI.conf" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <r>
       <rPr>
@@ -235,12 +236,6 @@
     <t>catalog=020F</t>
   </si>
   <si>
-    <t>kind=195000</t>
-  </si>
-  <si>
-    <t>catalog=020D</t>
-  </si>
-  <si>
     <t>kind=193000</t>
   </si>
   <si>
@@ -259,12 +254,6 @@
     <t>catalog=0B03</t>
   </si>
   <si>
-    <t>kind=19020201</t>
-  </si>
-  <si>
-    <t>catalog=01ff01</t>
-  </si>
-  <si>
     <t>kind=190214</t>
   </si>
   <si>
@@ -321,10 +310,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>外国首都名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>大洋名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -334,10 +319,6 @@
   </si>
   <si>
     <t>海域名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>普通岛屿</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -356,8 +337,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,28 +368,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -444,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -458,14 +424,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -746,11 +709,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -761,18 +724,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -804,18 +767,18 @@
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>54</v>
+      <c r="C6" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -826,7 +789,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -837,7 +800,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -848,29 +811,29 @@
         <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>68</v>
+      <c r="C10" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>69</v>
+      <c r="C11" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -881,7 +844,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -892,7 +855,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -903,7 +866,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -914,7 +877,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -925,7 +888,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -936,7 +899,7 @@
         <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -947,18 +910,18 @@
         <v>35</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>62</v>
+      <c r="C19" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -969,7 +932,7 @@
         <v>39</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -980,7 +943,7 @@
         <v>41</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -991,40 +954,18 @@
         <v>43</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fxi some bug in config File
</commit_message>
<xml_diff>
--- a/conf/excel/B_China_POI.xlsx
+++ b/conf/excel/B_China_POI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\学习资料\综合学习资料\tencent\配置文件相关\newCA-config-clear\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\学习资料\综合学习资料\tencent\配置文件相关\newCA-config-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FA784C-A48A-48AF-88A5-0649004A9D9C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B7E118-C23A-42CD-A2B1-0B63B73A3733}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B_China_POI.conf" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <r>
       <rPr>
@@ -331,6 +331,18 @@
   </si>
   <si>
     <t>敏感岛屿（显示层级5）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kind=19020201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>catalog=01FF01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普通岛屿</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -710,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -948,23 +960,34 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>